<commit_message>
Modification des gabarits export questionnaire autodiag
</commit_message>
<xml_diff>
--- a/files/autodiag/questionnaire.xlsx
+++ b/files/autodiag/questionnaire.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Greg/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="chapitres" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>code_chapitre</t>
   </si>
@@ -68,6 +73,12 @@
   </si>
   <si>
     <t>ponderation_chapitre</t>
+  </si>
+  <si>
+    <t>ordre_chapitre</t>
+  </si>
+  <si>
+    <t>ordre_question</t>
   </si>
 </sst>
 </file>
@@ -183,6 +194,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -508,13 +524,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
@@ -525,51 +541,49 @@
     <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
@@ -583,44 +597,42 @@
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#6305 - Add child number column for ad chapters
</commit_message>
<xml_diff>
--- a/files/autodiag/questionnaire.xlsx
+++ b/files/autodiag/questionnaire.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26215"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Greg/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="chapitres" sheetId="1" r:id="rId1"/>
     <sheet name="questions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,30 +25,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>code_chapitre</t>
   </si>
   <si>
+    <t>ordre_chapitre</t>
+  </si>
+  <si>
+    <t>numero_chapitre</t>
+  </si>
+  <si>
     <t>libelle_chapitre</t>
   </si>
   <si>
     <t>code_chapitre_enfant</t>
   </si>
   <si>
+    <t>numero_chapitre_enfant</t>
+  </si>
+  <si>
     <t>libelle_chapitre_enfant</t>
   </si>
   <si>
+    <t>titre_avant</t>
+  </si>
+  <si>
     <t>texte_avant</t>
   </si>
   <si>
     <t>texte_apres</t>
   </si>
   <si>
+    <t>plan_action</t>
+  </si>
+  <si>
     <t>code_question</t>
   </si>
   <si>
-    <t>plan_action</t>
+    <t>ordre_question</t>
+  </si>
+  <si>
+    <t>numero_question</t>
   </si>
   <si>
     <t>libelle_question</t>
@@ -66,48 +84,21 @@
     <t>infobulle_question</t>
   </si>
   <si>
-    <t>titre_avant</t>
-  </si>
-  <si>
-    <t>ponderation_categorie</t>
+    <t>ponderation_categories</t>
   </si>
   <si>
     <t>ponderation_chapitre</t>
-  </si>
-  <si>
-    <t>ordre_chapitre</t>
-  </si>
-  <si>
-    <t>ordre_question</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,73 +118,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="29">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -203,9 +138,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Bureau">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -243,7 +178,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Bureau">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -315,7 +250,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Bureau">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -347,16 +282,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -478,161 +417,140 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#6665 - Adding unit for autodiag text responses
</commit_message>
<xml_diff>
--- a/files/autodiag/questionnaire.xlsx
+++ b/files/autodiag/questionnaire.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Sites/hopitalnumerique/files/autodiag/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>code_chapitre</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>ponderation_chapitre</t>
+  </si>
+  <si>
+    <t>unite_reponse</t>
   </si>
 </sst>
 </file>
@@ -488,11 +491,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -510,7 +511,7 @@
     <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -530,21 +531,24 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
6433 - Adding additional description for autodiag attributes
</commit_message>
<xml_diff>
--- a/files/autodiag/questionnaire.xlsx
+++ b/files/autodiag/questionnaire.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Sites/hopitalnumerique/files/autodiag/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620"/>
   </bookViews>
   <sheets>
     <sheet name="chapitres" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>code_chapitre</t>
   </si>
@@ -429,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -491,9 +491,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -503,15 +505,17 @@
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -531,24 +535,27 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>